<commit_message>
XLS, XLSX converters with Facade
</commit_message>
<xml_diff>
--- a/files/excel.xlsx
+++ b/files/excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/labelworx/packages/excel-converter/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF74EA88-B609-B140-B618-C9225C3A47DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E89FEAD9-EBFC-0646-AC17-F20BE2925BF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="82680" yWindow="10660" windowWidth="27240" windowHeight="16440" xr2:uid="{6C79C411-7FA7-5A4F-A71A-B7543BC6AFB1}"/>
+    <workbookView xWindow="77680" yWindow="13940" windowWidth="26840" windowHeight="15940" xr2:uid="{4F1EA942-031B-7044-A5B7-797AEE6EE579}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,45 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>two</t>
+  </si>
+  <si>
+    <t>three</t>
+  </si>
+  <si>
+    <t>four</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>Chris, Chambers</t>
+  </si>
+  <si>
+    <t>(0123) 123 3455</t>
+  </si>
+  <si>
+    <t>Some House</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00_);[Red]\(&quot;£&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="mm\-dd\-yyyy"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
@@ -69,11 +105,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,11 +424,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A8CBC1-F009-6A4E-AB7B-A1374D1F33CB}">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F33331E1-47B1-334E-9B46-D017E480BD22}">
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -400,165 +437,74 @@
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("IMPORTRANGE(""https://docs.google.com/spreadsheets/d/1a7orCZzpNUthD1fg22JocziPs6_K5lkS_PtPLCEjAko/edit#gid=0"",""Sheet1!A1:F100000"")"),"name")</f>
-        <v>name</v>
-      </c>
-      <c r="B1" s="1" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"normalised_name")</f>
-        <v>normalised_name</v>
-      </c>
-      <c r="C1" s="1" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"new_addition")</f>
-        <v>new_addition</v>
-      </c>
-      <c r="D1" s="1" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Can_be_approved")</f>
-        <v>Can_be_approved</v>
-      </c>
-      <c r="E1" s="1" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"artist_uri")</f>
-        <v>artist_uri</v>
-      </c>
-      <c r="F1" s="1" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"added_date")</f>
-        <v>added_date</v>
-      </c>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Mc Davi")</f>
-        <v>Mc Davi</v>
-      </c>
-      <c r="B2" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"mcdavi")</f>
-        <v>mcdavi</v>
-      </c>
-      <c r="C2" s="2" t="b">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),TRUE)</f>
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="b">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),TRUE)</f>
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"spotify:artist:1cYhx7ZOhYoVmnDPb9KMwo")</f>
-        <v>spotify:artist:1cYhx7ZOhYoVmnDPb9KMwo</v>
-      </c>
-      <c r="F2" s="3">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44034)</f>
-        <v>44034</v>
-      </c>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Julion Alvarez")</f>
-        <v>Julion Alvarez</v>
-      </c>
-      <c r="B3" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"julionalvarez")</f>
-        <v>julionalvarez</v>
-      </c>
-      <c r="C3" s="2" t="b">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),TRUE)</f>
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="b">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"spotify:artist:6hawG2i16WnvEEqfDiv4we")</f>
-        <v>spotify:artist:6hawG2i16WnvEEqfDiv4we</v>
-      </c>
-      <c r="F3" s="3">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44034)</f>
-        <v>44034</v>
-      </c>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4">
+        <v>3.56</v>
+      </c>
+      <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"J Alvarez Banda Norteña")</f>
-        <v>J Alvarez Banda Norteña</v>
-      </c>
-      <c r="B4" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"jalvarezbandanortena")</f>
-        <v>jalvarezbandanortena</v>
-      </c>
-      <c r="C4" s="2" t="b">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),TRUE)</f>
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="b">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="E4" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"spotify:artist:1x0UGhijHGBX0bhm9ulj0y")</f>
-        <v>spotify:artist:1x0UGhijHGBX0bhm9ulj0y</v>
-      </c>
-      <c r="F4" s="3">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44034)</f>
-        <v>44034</v>
-      </c>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"El norteno de Julions")</f>
-        <v>El norteno de Julions</v>
-      </c>
-      <c r="B5" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"nortenojulions")</f>
-        <v>nortenojulions</v>
-      </c>
-      <c r="C5" s="2" t="b">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),TRUE)</f>
-        <v>1</v>
-      </c>
-      <c r="D5" s="2" t="b">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"spotify:artist:3ZY6NLBQz848Tvqepscord")</f>
-        <v>spotify:artist:3ZY6NLBQz848Tvqepscord</v>
-      </c>
-      <c r="F5" s="3">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44034)</f>
-        <v>44034</v>
-      </c>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Julion Alvarez ft Hansen Flores")</f>
-        <v>Julion Alvarez ft Hansen Flores</v>
-      </c>
-      <c r="B6" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"julionalvarezfthansenflores")</f>
-        <v>julionalvarezfthansenflores</v>
-      </c>
-      <c r="C6" s="2" t="b">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),TRUE)</f>
-        <v>1</v>
-      </c>
-      <c r="D6" s="2" t="b">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"spotify:artist:4uAmNfCsWQv8F1posVtgpV")</f>
-        <v>spotify:artist:4uAmNfCsWQv8F1posVtgpV</v>
-      </c>
-      <c r="F6" s="3">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44034)</f>
-        <v>44034</v>
-      </c>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
XLSX export specified worksheet
</commit_message>
<xml_diff>
--- a/files/excel.xlsx
+++ b/files/excel.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/labelworx/packages/excel-converter/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{37AB993F-D3CB-9144-982D-C4B886255BD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8799106-FA43-1B4E-9FF9-3AD6D6750C0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="77680" yWindow="13940" windowWidth="26840" windowHeight="15940" xr2:uid="{4F1EA942-031B-7044-A5B7-797AEE6EE579}"/>
+    <workbookView xWindow="75980" yWindow="15420" windowWidth="26840" windowHeight="15940" activeTab="2" xr2:uid="{4F1EA942-031B-7044-A5B7-797AEE6EE579}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Another Sheet" sheetId="2" r:id="rId2"/>
+    <sheet name="Third Sheet" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>one</t>
   </si>
@@ -58,6 +60,18 @@
   </si>
   <si>
     <t>boo</t>
+  </si>
+  <si>
+    <t>pink</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>purple</t>
+  </si>
+  <si>
+    <t>something</t>
   </si>
 </sst>
 </file>
@@ -429,11 +443,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F33331E1-47B1-334E-9B46-D017E480BD22}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -504,19 +516,60 @@
       </c>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B6AE5B0-ACF9-FE45-A558-08307C79C1F0}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E309D05-521C-824D-8B1D-7A7E8059EC29}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add exportDateFormat() option for XLS/XLSX files to ensure dates are formatted correctly for PHP
</commit_message>
<xml_diff>
--- a/files/excel.xlsx
+++ b/files/excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/labelworx/packages/excel-converter/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8799106-FA43-1B4E-9FF9-3AD6D6750C0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53DFBBC5-8F1D-1645-B04B-9DBBC625EAA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75980" yWindow="15420" windowWidth="26840" windowHeight="15940" activeTab="2" xr2:uid="{4F1EA942-031B-7044-A5B7-797AEE6EE579}"/>
+    <workbookView xWindow="33540" yWindow="18260" windowWidth="26840" windowHeight="15940" xr2:uid="{4F1EA942-031B-7044-A5B7-797AEE6EE579}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>one</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>something</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -82,7 +85,7 @@
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00_);[Red]\(&quot;£&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="mm\-dd\-yyyy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -95,11 +98,21 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -122,13 +135,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,7 +460,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F33331E1-47B1-334E-9B46-D017E480BD22}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -469,7 +486,9 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
+      <c r="E1" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -484,7 +503,9 @@
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="7">
+        <v>44044</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -499,7 +520,9 @@
       <c r="D3" s="4">
         <v>3.56</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="7">
+        <v>44044</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
@@ -560,7 +583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E309D05-521C-824D-8B1D-7A7E8059EC29}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Remove new lines from cells which broken CSV layouts
</commit_message>
<xml_diff>
--- a/files/excel.xlsx
+++ b/files/excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/labelworx/packages/excel-converter/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/labelworx/www/excel-converter/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53DFBBC5-8F1D-1645-B04B-9DBBC625EAA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068C6A1B-6190-5E4D-8A5A-6C9FABDB3EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33540" yWindow="18260" windowWidth="26840" windowHeight="15940" xr2:uid="{4F1EA942-031B-7044-A5B7-797AEE6EE579}"/>
+    <workbookView xWindow="33320" yWindow="16740" windowWidth="26840" windowHeight="15940" xr2:uid="{4F1EA942-031B-7044-A5B7-797AEE6EE579}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,9 +50,6 @@
     <t>blue</t>
   </si>
   <si>
-    <t>Chris, Chambers</t>
-  </si>
-  <si>
     <t>(0123) 123 3455</t>
   </si>
   <si>
@@ -75,6 +72,10 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>Chris,
+Chambers</t>
   </si>
 </sst>
 </file>
@@ -135,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -144,6 +145,9 @@
     <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,7 +465,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -487,7 +491,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -507,15 +511,15 @@
         <v>44044</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="D3" s="4">
         <v>3.56</v>
@@ -535,7 +539,7 @@
         <v>43831.965381944443</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="3"/>
     </row>
@@ -554,7 +558,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
@@ -565,10 +569,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -591,7 +595,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Parse cell formulas to just export raw value
</commit_message>
<xml_diff>
--- a/files/excel.xlsx
+++ b/files/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/labelworx/www/excel-converter/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068C6A1B-6190-5E4D-8A5A-6C9FABDB3EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB1BD71-2A7E-4347-8E29-6AF5231DEBF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33320" yWindow="16740" windowWidth="26840" windowHeight="15940" xr2:uid="{4F1EA942-031B-7044-A5B7-797AEE6EE579}"/>
   </bookViews>
@@ -22,12 +22,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>one</t>
   </si>
@@ -465,7 +476,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -504,8 +515,9 @@
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
+      <c r="D2" s="2" t="str">
+        <f>"bl" &amp; "ue"</f>
+        <v>blue</v>
       </c>
       <c r="E2" s="7">
         <v>44044</v>

</xml_diff>

<commit_message>
Excel Time Colum Fix
</commit_message>
<xml_diff>
--- a/files/excel.xlsx
+++ b/files/excel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/labelworx/www/excel-converter/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D639CB-AA95-7747-B40A-0DF7749F851C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DB4816-DF1E-6641-87AD-5D805ED5D4C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26520" yWindow="6060" windowWidth="26840" windowHeight="15940" xr2:uid="{4F1EA942-031B-7044-A5B7-797AEE6EE579}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>one</t>
   </si>
@@ -87,6 +87,9 @@
   <si>
     <t>Chris,
 Chambers</t>
+  </si>
+  <si>
+    <t>Time Format</t>
   </si>
 </sst>
 </file>
@@ -147,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -159,6 +162,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -177,9 +181,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -217,7 +221,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -323,7 +327,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -465,7 +469,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -473,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F33331E1-47B1-334E-9B46-D017E480BD22}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -554,6 +558,14 @@
         <v>9</v>
       </c>
       <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="9">
+        <v>0.12934027777777779</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>